<commit_message>
added IComparers for IBox interface
</commit_message>
<xml_diff>
--- a/SheetMetalArranger/ArrangerLibrary/Class diagram/Design.xlsx
+++ b/SheetMetalArranger/ArrangerLibrary/Class diagram/Design.xlsx
@@ -740,7 +740,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="114">
   <si>
     <t>int</t>
   </si>
@@ -1084,6 +1084,18 @@
   </si>
   <si>
     <t>mergeVertical</t>
+  </si>
+  <si>
+    <t>BoxHeightComparer</t>
+  </si>
+  <si>
+    <t>:IComparer&lt;IBox&gt;</t>
+  </si>
+  <si>
+    <t>BoxWidthComparer</t>
+  </si>
+  <si>
+    <t>BoxAreaComparer</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1401,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1397,7 +1408,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1433,24 +1443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1467,7 +1460,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dobre" xfId="2" builtinId="26"/>
@@ -1773,16 +1785,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M28" workbookViewId="0">
-      <selection activeCell="V49" sqref="V49"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="29.140625" bestFit="1" customWidth="1"/>
@@ -1799,51 +1811,51 @@
       <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="70" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="13"/>
-      <c r="E2" s="50">
+      <c r="E2" s="48">
         <v>1</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="50">
+      <c r="I2" s="21"/>
+      <c r="J2" s="48">
         <v>1</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="50">
+      <c r="N2" s="32"/>
+      <c r="O2" s="48">
         <v>1</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="50">
+      <c r="S2" s="32"/>
+      <c r="T2" s="48">
         <v>1</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="33" t="s">
+      <c r="W2" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="28">
+      <c r="X2" s="21"/>
+      <c r="Y2" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1854,7 +1866,7 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1872,7 +1884,7 @@
       <c r="M3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="7" t="s">
@@ -1881,7 +1893,7 @@
       <c r="R3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S3" s="16" t="s">
         <v>7</v>
       </c>
       <c r="V3" s="1" t="s">
@@ -1913,31 +1925,31 @@
       <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="35" t="s">
+      <c r="Q4" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="37" t="s">
+      <c r="S4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="W4" s="30" t="s">
+      <c r="W4" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="X4" s="31" t="s">
+      <c r="X4" s="29" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1960,31 +1972,31 @@
       <c r="I5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="35" t="s">
+      <c r="Q5" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="37" t="s">
+      <c r="S5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="29" t="s">
+      <c r="V5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="W5" s="30" t="s">
+      <c r="W5" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="X5" s="31" t="s">
+      <c r="X5" s="29" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2007,42 +2019,42 @@
       <c r="I6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="36" t="s">
+      <c r="Q6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="37" t="s">
+      <c r="S6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="V6" s="62" t="s">
+      <c r="V6" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="W6" s="60" t="s">
+      <c r="W6" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="X6" s="58" t="s">
+      <c r="X6" s="64" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="39" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -2054,109 +2066,110 @@
       <c r="I7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="68" t="s">
+      <c r="L7" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="66" t="s">
+      <c r="M7" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="64" t="s">
+      <c r="N7" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="38" t="s">
+      <c r="Q7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="R7" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="39" t="s">
+      <c r="S7" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="V7" s="62"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="58"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="64"/>
     </row>
     <row r="8" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="69"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="65"/>
-      <c r="Q8" s="38" t="s">
+      <c r="L8" s="62"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="58"/>
+      <c r="Q8" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="S8" s="39" t="s">
+      <c r="S8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="V8" s="63"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="59"/>
+      <c r="V8" s="68"/>
+      <c r="W8" s="66"/>
+      <c r="X8" s="65"/>
     </row>
     <row r="9" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L9" s="69"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="65"/>
-      <c r="Q9" s="38" t="s">
+      <c r="L9" s="62"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="58"/>
+      <c r="Q9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="R9" s="32" t="s">
+      <c r="R9" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="S9" s="39" t="s">
+      <c r="S9" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="24" t="s">
+      <c r="C10" s="69"/>
+      <c r="G10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="50">
+      <c r="J10" s="48">
         <v>1</v>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="39" t="s">
+      <c r="N10" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="35" t="s">
+      <c r="Q10" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="S10" s="37" t="s">
+      <c r="S10" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="V10" s="24" t="s">
+      <c r="V10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="W10" s="25" t="s">
+      <c r="W10" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="X10" s="26" t="s">
+      <c r="X10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="Y10" s="28">
+      <c r="Y10" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2167,34 +2180,34 @@
       <c r="H11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="L11" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="M11" s="51" t="s">
+      <c r="M11" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="N11" s="41" t="s">
+      <c r="N11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="Q11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" s="54" t="s">
+      <c r="Q11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="S11" s="55" t="s">
+      <c r="S11" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="V11" s="47" t="s">
+      <c r="V11" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="W11" s="48" t="s">
+      <c r="W11" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="X11" s="49" t="s">
+      <c r="X11" s="47" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2208,13 +2221,13 @@
       <c r="I12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V12" s="29" t="s">
+      <c r="V12" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="W12" s="30" t="s">
+      <c r="W12" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="X12" s="31" t="s">
+      <c r="X12" s="29" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2228,13 +2241,13 @@
       <c r="I13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="V13" s="29" t="s">
+      <c r="V13" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="W13" s="30" t="s">
+      <c r="W13" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="X13" s="31" t="s">
+      <c r="X13" s="29" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2248,13 +2261,13 @@
       <c r="I14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V14" s="62" t="s">
+      <c r="V14" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="W14" s="60" t="s">
+      <c r="W14" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="X14" s="64" t="s">
+      <c r="X14" s="57" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2268,44 +2281,44 @@
       <c r="I15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V15" s="62"/>
-      <c r="W15" s="60"/>
-      <c r="X15" s="64"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="63"/>
+      <c r="X15" s="57"/>
     </row>
     <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="24" t="s">
+      <c r="Q16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="R16" s="25" t="s">
+      <c r="R16" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="S16" s="26" t="s">
+      <c r="S16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="T16" s="50">
+      <c r="T16" s="48">
         <v>1</v>
       </c>
-      <c r="V16" s="62"/>
-      <c r="W16" s="60"/>
-      <c r="X16" s="64"/>
+      <c r="V16" s="67"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="57"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q17" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="48" t="s">
+      <c r="Q17" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="S17" s="57" t="s">
+      <c r="S17" s="55" t="s">
         <v>7</v>
       </c>
       <c r="V17" s="4" t="s">
@@ -2317,16 +2330,16 @@
       <c r="X17" s="6"/>
     </row>
     <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="50">
+      <c r="E18" s="48">
         <v>1</v>
       </c>
       <c r="Q18" s="1" t="s">
@@ -2349,37 +2362,37 @@
       <c r="D19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="J19" s="50">
+      <c r="J19" s="48">
         <v>1</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="L19" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="25" t="s">
+      <c r="M19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="N19" s="26" t="s">
+      <c r="N19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="O19" s="50">
+      <c r="O19" s="48">
         <v>1</v>
       </c>
-      <c r="Q19" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="R19" s="35" t="s">
+      <c r="Q19" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="S19" s="42" t="s">
+      <c r="S19" s="40" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2411,13 +2424,13 @@
       <c r="N20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="36" t="s">
+      <c r="Q20" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="R20" s="35" t="s">
+      <c r="R20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="S20" s="42" t="s">
+      <c r="S20" s="40" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2440,22 +2453,22 @@
       <c r="I21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="L21" s="29" t="s">
+      <c r="L21" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M21" s="30" t="s">
+      <c r="M21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="31" t="s">
+      <c r="N21" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="38" t="s">
+      <c r="Q21" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R21" s="32" t="s">
+      <c r="R21" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="S21" s="31" t="s">
+      <c r="S21" s="29" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2469,26 +2482,26 @@
       <c r="D22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="29" t="s">
+      <c r="L22" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="30" t="s">
+      <c r="M22" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="N22" s="31" t="s">
+      <c r="N22" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="38" t="s">
+      <c r="Q22" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="R22" s="32" t="s">
+      <c r="R22" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="S22" s="39" t="s">
+      <c r="S22" s="37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2498,24 +2511,24 @@
       <c r="D23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="29" t="s">
+      <c r="L23" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="36" t="s">
+      <c r="Q23" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="R23" s="35" t="s">
+      <c r="R23" s="33" t="s">
         <v>83</v>
       </c>
       <c r="S23" s="3"/>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2525,24 +2538,36 @@
       <c r="D24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="68" t="s">
+      <c r="G24" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24" s="48">
+        <v>1</v>
+      </c>
+      <c r="L24" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="60" t="s">
+      <c r="M24" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="64" t="s">
+      <c r="N24" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="Q24" s="36" t="s">
+      <c r="Q24" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="R24" s="35" t="s">
+      <c r="R24" s="33" t="s">
         <v>42</v>
       </c>
       <c r="S24" s="3"/>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
@@ -2552,268 +2577,323 @@
       <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="68"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="64"/>
-      <c r="Q25" s="38" t="s">
+      <c r="G25" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25" s="61"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="57"/>
+      <c r="Q25" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="R25" s="56" t="s">
+      <c r="R25" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="S25" s="39" t="s">
+      <c r="S25" s="37" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="L26" s="68"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="64"/>
-      <c r="Q26" s="38" t="s">
+      <c r="L26" s="61"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="57"/>
+      <c r="Q26" s="36" t="s">
         <v>88</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S26" s="39" t="s">
+      <c r="S26" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J27" s="48">
+        <v>1</v>
+      </c>
       <c r="L27" s="1" t="s">
         <v>63</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N27" s="37" t="s">
+      <c r="N27" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="Q27" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="R27" s="35" t="s">
+      <c r="Q27" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="S27" s="37" t="s">
+      <c r="S27" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="L28" s="38" t="s">
+    <row r="28" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="M28" s="32" t="s">
+      <c r="M28" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="N28" s="39" t="s">
+      <c r="N28" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="R28" s="35" t="s">
+      <c r="Q28" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="S28" s="37" t="s">
+      <c r="S28" s="35" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="29" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L29" s="40" t="s">
+      <c r="L29" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="M29" s="51" t="s">
+      <c r="M29" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="N29" s="41" t="s">
+      <c r="N29" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="Q29" s="40" t="s">
+      <c r="Q29" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="R29" s="51" t="s">
+      <c r="R29" s="49" t="s">
         <v>92</v>
       </c>
       <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q33" s="21" t="s">
+      <c r="Q33" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="R33" s="33" t="s">
+      <c r="R33" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="S33" s="23"/>
-      <c r="T33" s="50">
+      <c r="S33" s="21"/>
+      <c r="T33" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q34" s="43" t="s">
+      <c r="Q34" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="R34" s="44" t="s">
+      <c r="R34" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="S34" s="45" t="s">
+      <c r="S34" s="43" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q36" s="24" t="s">
+      <c r="Q36" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="R36" s="25" t="s">
+      <c r="R36" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="S36" s="26" t="s">
+      <c r="S36" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="T36" s="50">
+      <c r="T36" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q37" s="18" t="s">
+      <c r="Q37" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="R37" s="27" t="s">
+      <c r="R37" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="S37" s="20" t="s">
+      <c r="S37" s="19" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="38" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L38" s="24" t="s">
+      <c r="L38" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M38" s="25" t="s">
+      <c r="M38" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="N38" s="26" t="s">
+      <c r="N38" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O38" s="50">
+      <c r="O38" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L39" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="M39" s="19" t="s">
+      <c r="L39" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M39" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="N39" s="20" t="s">
+      <c r="N39" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="Q39" s="24" t="s">
+      <c r="Q39" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="R39" s="25" t="s">
+      <c r="R39" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="S39" s="26" t="s">
+      <c r="S39" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="T39" s="50">
+      <c r="T39" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q40" s="18" t="s">
+      <c r="Q40" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="R40" s="27" t="s">
+      <c r="R40" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="S40" s="20" t="s">
+      <c r="S40" s="19" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="41" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L41" s="24" t="s">
+      <c r="L41" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M41" s="25" t="s">
+      <c r="M41" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="N41" s="26" t="s">
+      <c r="N41" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O41" s="50">
+      <c r="O41" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L42" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="M42" s="19" t="s">
+      <c r="L42" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M42" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="N42" s="20" t="s">
+      <c r="N42" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="43" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L44" s="24" t="s">
+      <c r="L44" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M44" s="25" t="s">
+      <c r="M44" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="N44" s="26" t="s">
+      <c r="N44" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="O44" s="50">
+      <c r="O44" s="48">
         <v>1</v>
       </c>
-      <c r="Q44" s="24" t="s">
+      <c r="Q44" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="R44" s="25" t="s">
+      <c r="R44" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="S44" s="26"/>
-      <c r="T44" s="50">
+      <c r="S44" s="24"/>
+      <c r="T44" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L45" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="M45" s="19" t="s">
+      <c r="L45" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M45" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="N45" s="20" t="s">
+      <c r="N45" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="Q45" s="36" t="s">
+      <c r="Q45" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="R45" s="35" t="s">
+      <c r="R45" s="33" t="s">
         <v>96</v>
       </c>
       <c r="S45" s="3"/>
     </row>
     <row r="46" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="Q46" s="36" t="s">
+      <c r="Q46" s="34" t="s">
         <v>80</v>
       </c>
       <c r="R46" s="2" t="s">
@@ -2822,21 +2902,21 @@
       <c r="S46" s="3"/>
     </row>
     <row r="47" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="Q47" s="38" t="s">
+      <c r="Q47" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="R47" s="70" t="s">
+      <c r="R47" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="S47" s="31" t="s">
+      <c r="S47" s="29" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="48" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="Q48" s="38" t="s">
+      <c r="Q48" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="R48" s="70" t="s">
+      <c r="R48" s="56" t="s">
         <v>101</v>
       </c>
       <c r="S48" s="3" t="s">
@@ -2844,63 +2924,63 @@
       </c>
     </row>
     <row r="49" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q49" s="29" t="s">
+      <c r="Q49" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="R49" s="70" t="s">
+      <c r="R49" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="S49" s="31" t="s">
+      <c r="S49" s="29" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q50" s="29" t="s">
+      <c r="Q50" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="R50" s="70" t="s">
+      <c r="R50" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="S50" s="31" t="s">
+      <c r="S50" s="29" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="51" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q51" s="29" t="s">
+      <c r="Q51" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="R51" s="70" t="s">
+      <c r="R51" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="S51" s="31" t="s">
+      <c r="S51" s="29" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="52" spans="17:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q52" s="18" t="s">
+      <c r="Q52" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="R52" s="27" t="s">
+      <c r="R52" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="S52" s="20" t="s">
+      <c r="S52" s="19" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="X6:X8"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="V14:V16"/>
+    <mergeCell ref="X14:X16"/>
+    <mergeCell ref="W14:W16"/>
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="N24:N26"/>
     <mergeCell ref="M24:M26"/>
     <mergeCell ref="L24:L26"/>
-    <mergeCell ref="X6:X8"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="V14:V16"/>
-    <mergeCell ref="X14:X16"/>
-    <mergeCell ref="W14:W16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
first working version of library; - individual maring & rotation setting for items - merging adjacent boxes - new result branch is created for each possible placement
</commit_message>
<xml_diff>
--- a/SheetMetalArranger/ArrangerLibrary/Class diagram/Design.xlsx
+++ b/SheetMetalArranger/ArrangerLibrary/Class diagram/Design.xlsx
@@ -21,7 +21,7 @@
     <author>Mic Kajzer</author>
   </authors>
   <commentList>
-    <comment ref="L5" authorId="0">
+    <comment ref="AH9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -29,7 +29,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Mic Kajzer:</t>
         </r>
@@ -38,51 +38,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-returns </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>true</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> if succesfully removed;
-returns </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <i/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>false</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> removal unsuccessful (f.i. item isn't present in collection)</t>
+constructor:
+public Assignment(IBox _box, IItem _item, bool _rotated)</t>
         </r>
       </text>
     </comment>
@@ -111,55 +71,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="W10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mic Kajzer:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Constructor
-Arrangement();</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mic Kajzer:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-return overall utilisation ratio</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="I13" authorId="0">
       <text>
         <r>
@@ -204,7 +115,67 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-checks if an item can fit into container</t>
+checks if an item can fit into container;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>returns 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> if a box can hold given item without rotation
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>returns 2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> if a box can hold given item if rotated
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>returns 0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> if a box is not sufficient to hold given item</t>
         </r>
       </text>
     </comment>
@@ -228,8 +199,81 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Constructor:
-Sheet(int _h, int _w);</t>
+Constructors:
+public Panel(int _height, int _width);
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>private</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Panel(int _height, int _width, List&lt;IBox&gt; _boxes, List&lt;IAssignment&gt; _assignments);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Constructor
+Arrangement();</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Constructors:
+public Calculation(IBatch _batch, int _newHeight, int _newWidth);
+public Calculation(IBatch _batch, IPanel _defaultPanel);
+public Calculation(IBatch _batch, List&lt;IPanel&gt; _panels);
+public Calculation(IBatch _batch, List&lt;IPanel&gt; _panels, int _newHeight, int _newWidth);</t>
         </r>
       </text>
     </comment>
@@ -284,6 +328,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="H19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M19" authorId="0">
       <text>
         <r>
@@ -334,6 +402,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="X19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+return overall utilisation ratio</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D20" authorId="0">
       <text>
         <r>
@@ -430,6 +522,93 @@
         </r>
       </text>
     </comment>
+    <comment ref="M22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+returns </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>true</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> if given item is present in collection and has been succesfully removed
+returns </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>false</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> if given item isn't present in collection</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="R25" authorId="0">
       <text>
         <r>
@@ -451,6 +630,111 @@
           </rPr>
           <t xml:space="preserve">
 merge containers where possible</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+returns new instance of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arrangement</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> class with content of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">panels </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">and </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>leftItems</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> copied</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
         </r>
       </text>
     </comment>
@@ -487,6 +771,34 @@
           </rPr>
           <t>List&lt;Iitem&gt;content</t>
         </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> to avoid; this method does not return reference to actual </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>content</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> list (which is private) to avoid accessing all possible methods and properties which are public for generic list</t>
+        </r>
       </text>
     </comment>
     <comment ref="Q29" authorId="0">
@@ -543,7 +855,104 @@
         </r>
       </text>
     </comment>
-    <comment ref="R37" authorId="0">
+    <comment ref="H30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Constructor:
+public PossibleFit(IBox _box, IItem _item, IPanel _mother, bool _rotated, int _panelIndex);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +976,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="R40" authorId="0">
+    <comment ref="M41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+constructor private</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R42" authorId="0">
       <text>
         <r>
           <rPr>
@@ -591,7 +1048,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R47" authorId="0">
+    <comment ref="M44" authorId="0">
       <text>
         <r>
           <rPr>
@@ -611,11 +1068,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-returns list of boxes after all possible extensions</t>
+constructor private</t>
         </r>
       </text>
     </comment>
-    <comment ref="R48" authorId="0">
+    <comment ref="M47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -635,7 +1092,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-iterates through input and finds if a given box can be extended; iteration stops when all possible extensions have been performed</t>
+constructor private</t>
         </r>
       </text>
     </comment>
@@ -659,7 +1116,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-checks if two given boxes extend each other horizontally</t>
+returns list of boxes after all possible extensions</t>
         </r>
       </text>
     </comment>
@@ -683,7 +1140,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-checks if two given boxes extend each other vertically</t>
+iterates through input and finds if a given box can be extended; iteration stops when all possible extensions have been performed</t>
         </r>
       </text>
     </comment>
@@ -707,11 +1164,59 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-returns a box genereted by merging horizontally two given boxes</t>
+checks if two given boxes extend each other horizontally</t>
         </r>
       </text>
     </comment>
     <comment ref="R52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+checks if two given boxes extend each other vertically</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mic Kajzer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+returns a box genereted by merging horizontally two given boxes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -740,7 +1245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="171">
   <si>
     <t>int</t>
   </si>
@@ -829,9 +1334,6 @@
     <t>content</t>
   </si>
   <si>
-    <t>private</t>
-  </si>
-  <si>
     <t>singleton Class</t>
   </si>
   <si>
@@ -898,15 +1400,6 @@
     <t>Arrangement</t>
   </si>
   <si>
-    <t>Calculate</t>
-  </si>
-  <si>
-    <t>private IBatch</t>
-  </si>
-  <si>
-    <t>inputBatch</t>
-  </si>
-  <si>
     <t>Margin</t>
   </si>
   <si>
@@ -994,19 +1487,10 @@
     <t>boxes</t>
   </si>
   <si>
-    <t>(IBox _box, Iitem _item, ISector _sector)</t>
-  </si>
-  <si>
-    <t>(Ibox _box, Iitem _item, ISector _sector)</t>
-  </si>
-  <si>
     <t>merge</t>
   </si>
   <si>
     <t>GetBox</t>
-  </si>
-  <si>
-    <t>public IBox</t>
   </si>
   <si>
     <t>AvailableBoxes</t>
@@ -1097,6 +1581,198 @@
   <si>
     <t>BoxAreaComparer</t>
   </si>
+  <si>
+    <t>ICalculation</t>
+  </si>
+  <si>
+    <t>AddPanel</t>
+  </si>
+  <si>
+    <t>(IPanel _panel)</t>
+  </si>
+  <si>
+    <t>GetLeftItems</t>
+  </si>
+  <si>
+    <t>LeaveItem</t>
+  </si>
+  <si>
+    <t>AddPanels</t>
+  </si>
+  <si>
+    <t>(List&lt;IPanel&gt; _panels</t>
+  </si>
+  <si>
+    <t>:IComparer&lt;IArrangement&gt;</t>
+  </si>
+  <si>
+    <t>(IArrangement _item1, IArrangement _item2)</t>
+  </si>
+  <si>
+    <t>private List&lt;IPanel&gt;</t>
+  </si>
+  <si>
+    <t>panels</t>
+  </si>
+  <si>
+    <t>private List&lt;IItem&gt;</t>
+  </si>
+  <si>
+    <t>leftItems</t>
+  </si>
+  <si>
+    <t>NewBranch</t>
+  </si>
+  <si>
+    <t>IArrangementRatioComparer</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>:ICalculation</t>
+  </si>
+  <si>
+    <t>inputBatch</t>
+  </si>
+  <si>
+    <t>private IBatch</t>
+  </si>
+  <si>
+    <t>arrangements</t>
+  </si>
+  <si>
+    <t>private List&lt;IArrangements&gt;</t>
+  </si>
+  <si>
+    <t>allowNewPanels</t>
+  </si>
+  <si>
+    <t>private int</t>
+  </si>
+  <si>
+    <t>defaultHeight</t>
+  </si>
+  <si>
+    <t>defaultWidth</t>
+  </si>
+  <si>
+    <t>private readonly PossibleFitComparer</t>
+  </si>
+  <si>
+    <t>fitComparer</t>
+  </si>
+  <si>
+    <t>Calculate</t>
+  </si>
+  <si>
+    <t>(IComparer&lt;IItem&gt; _item1comparer, IComparer&lt;IItem&gt; _item2comparer, IComparer&lt;IItem&gt; _item3comparer, ISector _sector)</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>OutputString</t>
+  </si>
+  <si>
+    <t>OutputBest</t>
+  </si>
+  <si>
+    <t>private List&lt;PossibleFit&gt;</t>
+  </si>
+  <si>
+    <t>findPossibleFits</t>
+  </si>
+  <si>
+    <t>(IItem _item, IArrangement _arrangement)</t>
+  </si>
+  <si>
+    <t>PossibleFit</t>
+  </si>
+  <si>
+    <t>sub-class of Calculation</t>
+  </si>
+  <si>
+    <t>private sealed class</t>
+  </si>
+  <si>
+    <t>UsedBox</t>
+  </si>
+  <si>
+    <t>get; private set;</t>
+  </si>
+  <si>
+    <t>PlacedItem</t>
+  </si>
+  <si>
+    <t>MotherPanel</t>
+  </si>
+  <si>
+    <t>AreaRatio</t>
+  </si>
+  <si>
+    <t>Rotated</t>
+  </si>
+  <si>
+    <t>PanelIndex</t>
+  </si>
+  <si>
+    <t>PossibleFitAreaComparer</t>
+  </si>
+  <si>
+    <t>:IComparer&lt;PossibleFit&gt;</t>
+  </si>
+  <si>
+    <t>(PossibleFit _fit1, PossibleFit _fit2)</t>
+  </si>
+  <si>
+    <t>singleton sealed Class</t>
+  </si>
+  <si>
+    <t>ItemEquality</t>
+  </si>
+  <si>
+    <t>:IEqualityComparer &lt;IItem&gt;</t>
+  </si>
+  <si>
+    <t>(IItem x, IItem y)</t>
+  </si>
+  <si>
+    <t>(IItem obj)</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>IAssignment</t>
+  </si>
+  <si>
+    <t>:IAssignemnt</t>
+  </si>
+  <si>
+    <t>get; private set</t>
+  </si>
+  <si>
+    <t>List&lt;IAssignment&gt;</t>
+  </si>
+  <si>
+    <t>Assignments</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>(Ibox _box, Iitem _item, ISector _sector, bool _rotated)</t>
+  </si>
+  <si>
+    <t>(IBox _box, Iitem _item, ISector _sector, bool _rotated)</t>
+  </si>
 </sst>
 </file>
 
@@ -1106,13 +1782,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1224,18 +1893,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1381,12 +2052,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1396,95 +2066,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Dobre" xfId="2" builtinId="26"/>
+  <cellStyles count="2">
+    <cellStyle name="Dobre" xfId="1" builtinId="26"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Złe" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1783,83 +2480,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Y52"/>
+  <dimension ref="B1:AJ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="24.42578125" customWidth="1"/>
-    <col min="19" max="19" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" customWidth="1"/>
-    <col min="24" max="24" width="32.28515625" customWidth="1"/>
+    <col min="19" max="19" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="41.140625" customWidth="1"/>
+    <col min="33" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="55" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="13"/>
-      <c r="E2" s="48">
+      <c r="E2" s="46">
         <v>1</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>58</v>
+      <c r="H2" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="I2" s="21"/>
-      <c r="J2" s="48">
+      <c r="J2" s="46">
         <v>1</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="48">
+      <c r="N2" s="31"/>
+      <c r="O2" s="46">
         <v>1</v>
       </c>
       <c r="Q2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="48">
+      <c r="R2" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="31"/>
+      <c r="T2" s="46">
         <v>1</v>
       </c>
       <c r="V2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="31" t="s">
-        <v>49</v>
+      <c r="W2" s="30" t="s">
+        <v>48</v>
       </c>
       <c r="X2" s="21"/>
-      <c r="Y2" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Y2" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="46">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH2" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1896,17 +2619,35 @@
       <c r="S3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AA3" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB3" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC3" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1925,35 +2666,48 @@
       <c r="I4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="33" t="s">
+      <c r="Q4" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="S4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="W4" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="X4" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="V4" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="X4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="29"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="75"/>
+      <c r="AG4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1972,35 +2726,48 @@
       <c r="I5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="29" t="s">
+      <c r="N5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="33" t="s">
+      <c r="Q5" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="V5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="W5" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="X5" s="29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="X5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="29"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="79"/>
+      <c r="AC5" s="75"/>
+      <c r="AG5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2019,43 +2786,46 @@
       <c r="I6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="Q6" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R6" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="V6" s="67" t="s">
+      <c r="V6" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="W6" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="X6" s="64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+      <c r="W6" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="X6" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA6" s="78"/>
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="75"/>
+    </row>
+    <row r="7" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>38</v>
+      <c r="C7" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>0</v>
@@ -2066,31 +2836,46 @@
       <c r="I7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="61" t="s">
+      <c r="L7" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="59" t="s">
+      <c r="M7" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="57" t="s">
+      <c r="N7" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="36" t="s">
+      <c r="Q7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="30" t="s">
+      <c r="R7" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="V7" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="X7" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="V7" s="67"/>
-      <c r="W7" s="63"/>
-      <c r="X7" s="64"/>
-    </row>
-    <row r="8" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA7" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB7" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC7" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G8" s="17" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>15</v>
@@ -2098,82 +2883,124 @@
       <c r="I8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="62"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="58"/>
-      <c r="Q8" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="R8" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="S8" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="V8" s="68"/>
-      <c r="W8" s="66"/>
-      <c r="X8" s="65"/>
-    </row>
-    <row r="9" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L9" s="62"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="58"/>
-      <c r="Q9" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="R9" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="S9" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="69"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="63"/>
+      <c r="Q8" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="S8" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="W8" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="X8" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB8" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC8" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="67"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="63"/>
+      <c r="Q9" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="S9" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="W9" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="X9" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH9" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI9" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ9" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="54"/>
       <c r="G10" s="22" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="48">
+        <v>55</v>
+      </c>
+      <c r="J10" s="46">
         <v>1</v>
       </c>
-      <c r="L10" s="36" t="s">
+      <c r="L10" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="N10" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="S10" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="V10" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="W10" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="X10" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y10" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="V10" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="W10" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="X10" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH10" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI10" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G11" s="7" t="s">
         <v>0</v>
       </c>
@@ -2183,35 +3010,35 @@
       <c r="I11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q11" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="S11" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="V11" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W11" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="47" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="L11" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="N11" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2221,17 +3048,26 @@
       <c r="I12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V12" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="W12" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="X12" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q12" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="R12" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="S12" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH12" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G13" s="1" t="s">
         <v>0</v>
       </c>
@@ -2241,17 +3077,17 @@
       <c r="I13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="V13" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="W13" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="X13" s="29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q13" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="R13" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="S13" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2261,17 +3097,8 @@
       <c r="I14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V14" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="W14" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="X14" s="57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2281,13 +3108,10 @@
       <c r="I15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V15" s="67"/>
-      <c r="W15" s="63"/>
-      <c r="X15" s="57"/>
-    </row>
-    <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G16" s="17" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H16" s="25" t="s">
         <v>15</v>
@@ -2296,50 +3120,78 @@
         <v>16</v>
       </c>
       <c r="Q16" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="T16" s="48">
+        <v>71</v>
+      </c>
+      <c r="T16" s="46">
         <v>1</v>
       </c>
-      <c r="V16" s="67"/>
-      <c r="W16" s="63"/>
-      <c r="X16" s="57"/>
-    </row>
-    <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q17" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="46" t="s">
+      <c r="V16" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="W16" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="X16" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y16" s="46">
         <v>1</v>
       </c>
-      <c r="S17" s="55" t="s">
+      <c r="AA16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB16" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD16" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q17" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="V17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="W17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="X17" s="6"/>
-    </row>
-    <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="W17" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="X17" s="16"/>
+      <c r="AA17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC17" s="3"/>
+    </row>
+    <row r="18" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="46">
         <v>1</v>
       </c>
       <c r="Q18" s="1" t="s">
@@ -2351,8 +3203,22 @@
       <c r="S18" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="X18" s="3"/>
+      <c r="AA18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC18" s="3"/>
+    </row>
+    <row r="19" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>0</v>
       </c>
@@ -2363,15 +3229,15 @@
         <v>2</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>30</v>
+        <v>155</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="48">
+        <v>63</v>
+      </c>
+      <c r="J19" s="46">
         <v>1</v>
       </c>
       <c r="L19" s="22" t="s">
@@ -2383,20 +3249,36 @@
       <c r="N19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="O19" s="48">
+      <c r="O19" s="46">
         <v>1</v>
       </c>
-      <c r="Q19" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R19" s="33" t="s">
+      <c r="Q19" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="S19" s="40" t="s">
+      <c r="S19" s="39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V19" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="W19" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="X19" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC19" s="3"/>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2406,14 +3288,14 @@
       <c r="D20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>69</v>
+      <c r="H20" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>65</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>0</v>
@@ -2424,17 +3306,33 @@
       <c r="N20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="34" t="s">
+      <c r="Q20" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="R20" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="S20" s="40" t="s">
+      <c r="S20" s="39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V20" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="W20" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="X20" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA20" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB20" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC20" s="3"/>
+    </row>
+    <row r="21" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2444,35 +3342,51 @@
       <c r="D21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L21" s="27" t="s">
+      <c r="G21" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M21" s="28" t="s">
+      <c r="M21" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="29" t="s">
+      <c r="N21" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="36" t="s">
+      <c r="Q21" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="R21" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="S21" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="R21" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="V21" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="W21" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="X21" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA21" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB21" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC21" s="3"/>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
@@ -2482,97 +3396,143 @@
       <c r="D22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="27" t="s">
+      <c r="L22" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="28" t="s">
+      <c r="M22" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="N22" s="29" t="s">
+      <c r="N22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="R22" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="S22" s="37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q22" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="R22" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="S22" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="V22" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="W22" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="X22" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA22" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB22" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC22" s="3"/>
+    </row>
+    <row r="23" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="27" t="s">
+      <c r="L23" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M23" s="28" t="s">
+      <c r="M23" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N23" s="29" t="s">
+      <c r="N23" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="R23" s="33" t="s">
-        <v>83</v>
+      <c r="Q23" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="R23" s="32" t="s">
+        <v>79</v>
       </c>
       <c r="S23" s="3"/>
-    </row>
-    <row r="24" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="W23" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="X23" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA23" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB23" s="76" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC23" s="75" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>30</v>
+        <v>155</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="J24" s="48">
+        <v>104</v>
+      </c>
+      <c r="J24" s="46">
         <v>1</v>
       </c>
-      <c r="L24" s="61" t="s">
+      <c r="L24" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="63" t="s">
+      <c r="M24" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="57" t="s">
+      <c r="N24" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="Q24" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="R24" s="33" t="s">
-        <v>42</v>
+      <c r="Q24" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="R24" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="S24" s="3"/>
-    </row>
-    <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V24" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="W24" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="X24" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA24" s="77"/>
+      <c r="AB24" s="76"/>
+      <c r="AC24" s="75"/>
+    </row>
+    <row r="25" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>7</v>
@@ -2581,400 +3541,610 @@
         <v>0</v>
       </c>
       <c r="H25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L25" s="61"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="57"/>
-      <c r="Q25" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="R25" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="S25" s="37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="38" t="s">
+      <c r="L25" s="66"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="62"/>
+      <c r="Q25" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="R25" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="S25" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="V25" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="W25" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="X25" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA25" s="77"/>
+      <c r="AB25" s="76"/>
+      <c r="AC25" s="75"/>
+    </row>
+    <row r="26" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="L26" s="61"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="57"/>
-      <c r="Q26" s="36" t="s">
-        <v>88</v>
+      <c r="C26" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="66"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="62"/>
+      <c r="Q26" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="S26" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="S26" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="V26" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="W26" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="X26" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA26" s="77"/>
+      <c r="AB26" s="76"/>
+      <c r="AC26" s="75"/>
+    </row>
+    <row r="27" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G27" s="22" t="s">
-        <v>30</v>
+        <v>155</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="J27" s="48">
+        <v>104</v>
+      </c>
+      <c r="J27" s="46">
         <v>1</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N27" s="35" t="s">
+      <c r="N27" s="34"/>
+      <c r="Q27" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="S27" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA27" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB27" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC27" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="N28" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="S28" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA28" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB28" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC28" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L29" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="M29" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="N29" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="S29" s="3"/>
+      <c r="AA29" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB29" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC29" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" s="46">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="R30" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="S30" s="80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q31" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="R31" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="S31" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA32" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB32" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC32" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD32" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V33" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q27" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R27" s="33" t="s">
+      <c r="W33" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="X33" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y33" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC33" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V34" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="W34" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X34" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA34" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB34" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC34" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="R35" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="S35" s="21"/>
+      <c r="T35" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB35" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="R36" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="S36" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA36" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB36" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC36" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA37" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB37" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC37" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L38" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="N38" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" s="46">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="R38" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="S38" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="T38" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC38" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q39" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="R39" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="S39" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="M41" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N41" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O41" s="46">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="R41" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S41" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="T41" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB41" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC41" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD41" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L42" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q42" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="R42" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="S42" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA42" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC42" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L44" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="M44" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N44" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O44" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L45" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M45" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q46" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="R46" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="S46" s="24"/>
+      <c r="T46" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="12:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L47" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="M47" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="N47" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="O47" s="46">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="R47" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="S27" s="35" t="s">
+      <c r="S47" s="3"/>
+    </row>
+    <row r="48" spans="12:30" x14ac:dyDescent="0.25">
+      <c r="L48" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="M48" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q48" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="R48" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L28" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="M28" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q28" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="R28" s="33" t="s">
+      <c r="S48" s="3"/>
+    </row>
+    <row r="49" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L49" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N49" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q49" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="R49" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="S28" s="35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L29" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="M29" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q29" s="38" t="s">
+      <c r="S49" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="Q50" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="R29" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="S29" s="6"/>
-    </row>
-    <row r="30" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="J30" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G31" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q33" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="R33" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="S33" s="21"/>
-      <c r="T33" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q34" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="R34" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="S34" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q36" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="R36" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="S36" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="T36" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q37" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="R37" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="S37" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L38" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="M38" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="N38" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O38" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L39" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M39" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="N39" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q39" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="R39" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="S39" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="T39" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q40" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="R40" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="S40" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L41" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="M41" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="N41" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O41" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M42" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="N42" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L44" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="M44" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="N44" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O44" s="48">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="22" t="s">
+      <c r="R50" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="R44" s="23" t="s">
+      <c r="S50" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="S44" s="24"/>
-      <c r="T44" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="12:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M45" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="N45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="R45" s="33" t="s">
+    </row>
+    <row r="51" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="Q51" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="R51" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="S45" s="3"/>
-    </row>
-    <row r="46" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="Q46" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="R46" s="2" t="s">
+      <c r="S51" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="S46" s="3"/>
-    </row>
-    <row r="47" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="Q47" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="R47" s="56" t="s">
+    </row>
+    <row r="52" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="Q52" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="R52" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="S47" s="29" t="s">
+      <c r="S52" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="Q53" s="26" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="48" spans="12:20" x14ac:dyDescent="0.25">
-      <c r="Q48" s="36" t="s">
+      <c r="R53" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="R48" s="56" t="s">
+      <c r="S53" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="S48" s="3" t="s">
+    </row>
+    <row r="54" spans="12:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q54" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="R54" s="25" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q49" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="R49" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="S49" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q50" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="R50" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="S50" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="17:19" x14ac:dyDescent="0.25">
-      <c r="Q51" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="R51" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="S51" s="29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="17:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q52" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="R52" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="S52" s="19" t="s">
-        <v>108</v>
+      <c r="S54" s="19" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="X6:X8"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="V14:V16"/>
-    <mergeCell ref="X14:X16"/>
-    <mergeCell ref="W14:W16"/>
+    <mergeCell ref="AC23:AC26"/>
+    <mergeCell ref="AB23:AB26"/>
+    <mergeCell ref="AA23:AA26"/>
+    <mergeCell ref="AC3:AC6"/>
+    <mergeCell ref="AB3:AB6"/>
+    <mergeCell ref="AA3:AA6"/>
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="L7:L9"/>

</xml_diff>

<commit_message>
demo works, added unit test to test calculation in ArrangerLibrary with specified set of panels and new panels allowed
</commit_message>
<xml_diff>
--- a/SheetMetalArranger/ArrangerLibrary/Class diagram/Design.xlsx
+++ b/SheetMetalArranger/ArrangerLibrary/Class diagram/Design.xlsx
@@ -2131,6 +2131,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2150,34 +2178,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dobre" xfId="1" builtinId="26"/>
@@ -2482,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AJ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="N26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N57" sqref="A57:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,13 +2628,13 @@
       <c r="X3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="AA3" s="78" t="s">
+      <c r="AA3" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="79" t="s">
+      <c r="AB3" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="AC3" s="75" t="s">
+      <c r="AC3" s="69" t="s">
         <v>135</v>
       </c>
       <c r="AG3" s="1" t="s">
@@ -2694,9 +2694,9 @@
         <v>37</v>
       </c>
       <c r="Y4" s="29"/>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="75"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="69"/>
       <c r="AG4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2754,9 +2754,9 @@
         <v>49</v>
       </c>
       <c r="Y5" s="29"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="79"/>
-      <c r="AC5" s="75"/>
+      <c r="AA5" s="73"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="69"/>
       <c r="AG5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2813,9 +2813,9 @@
       <c r="X6" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="79"/>
-      <c r="AC6" s="75"/>
+      <c r="AA6" s="73"/>
+      <c r="AB6" s="72"/>
+      <c r="AC6" s="69"/>
     </row>
     <row r="7" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="37" t="s">
@@ -2836,13 +2836,13 @@
       <c r="I7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="66" t="s">
+      <c r="L7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="62" t="s">
+      <c r="N7" s="74" t="s">
         <v>24</v>
       </c>
       <c r="Q7" s="35" t="s">
@@ -2883,9 +2883,9 @@
       <c r="I8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="67"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="63"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="75"/>
       <c r="Q8" s="35" t="s">
         <v>75</v>
       </c>
@@ -2915,9 +2915,9 @@
       </c>
     </row>
     <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L9" s="67"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="63"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="75"/>
       <c r="Q9" s="35" t="s">
         <v>54</v>
       </c>
@@ -2927,13 +2927,13 @@
       <c r="S9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="V9" s="69" t="s">
+      <c r="V9" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="W9" s="70" t="s">
+      <c r="W9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="X9" s="71" t="s">
+      <c r="X9" s="64" t="s">
         <v>113</v>
       </c>
       <c r="AG9" s="22" t="s">
@@ -3054,7 +3054,7 @@
       <c r="R12" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="S12" s="80" t="s">
+      <c r="S12" s="68" t="s">
         <v>83</v>
       </c>
       <c r="AG12" s="4" t="s">
@@ -3131,13 +3131,13 @@
       <c r="T16" s="46">
         <v>1</v>
       </c>
-      <c r="V16" s="72" t="s">
+      <c r="V16" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="W16" s="73" t="s">
+      <c r="W16" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="X16" s="74" t="s">
+      <c r="X16" s="67" t="s">
         <v>68</v>
       </c>
       <c r="Y16" s="46">
@@ -3466,13 +3466,13 @@
       <c r="X23" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AA23" s="77" t="s">
+      <c r="AA23" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="AB23" s="76" t="s">
+      <c r="AB23" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="AC23" s="75" t="s">
+      <c r="AC23" s="69" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3498,13 +3498,13 @@
       <c r="J24" s="46">
         <v>1</v>
       </c>
-      <c r="L24" s="66" t="s">
+      <c r="L24" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="68" t="s">
+      <c r="M24" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="62" t="s">
+      <c r="N24" s="74" t="s">
         <v>24</v>
       </c>
       <c r="Q24" s="33" t="s">
@@ -3514,18 +3514,18 @@
         <v>41</v>
       </c>
       <c r="S24" s="3"/>
-      <c r="V24" s="69" t="s">
+      <c r="V24" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="W24" s="70" t="s">
+      <c r="W24" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="X24" s="71" t="s">
+      <c r="X24" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="AA24" s="77"/>
-      <c r="AB24" s="76"/>
-      <c r="AC24" s="75"/>
+      <c r="AA24" s="71"/>
+      <c r="AB24" s="70"/>
+      <c r="AC24" s="69"/>
     </row>
     <row r="25" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
@@ -3546,9 +3546,9 @@
       <c r="I25" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="L25" s="66"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="62"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="74"/>
       <c r="Q25" s="35" t="s">
         <v>42</v>
       </c>
@@ -3567,9 +3567,9 @@
       <c r="X25" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="AA25" s="77"/>
-      <c r="AB25" s="76"/>
-      <c r="AC25" s="75"/>
+      <c r="AA25" s="71"/>
+      <c r="AB25" s="70"/>
+      <c r="AC25" s="69"/>
     </row>
     <row r="26" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="37" t="s">
@@ -3581,9 +3581,9 @@
       <c r="D26" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="L26" s="66"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="62"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="74"/>
       <c r="Q26" s="35" t="s">
         <v>54</v>
       </c>
@@ -3602,9 +3602,9 @@
       <c r="X26" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="AA26" s="77"/>
-      <c r="AB26" s="76"/>
-      <c r="AC26" s="75"/>
+      <c r="AA26" s="71"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="69"/>
     </row>
     <row r="27" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G27" s="22" t="s">
@@ -3729,7 +3729,7 @@
       <c r="R30" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="S30" s="80" t="s">
+      <c r="S30" s="68" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4139,18 +4139,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="N24:N26"/>
+    <mergeCell ref="M24:M26"/>
+    <mergeCell ref="L24:L26"/>
     <mergeCell ref="AC23:AC26"/>
     <mergeCell ref="AB23:AB26"/>
     <mergeCell ref="AA23:AA26"/>
     <mergeCell ref="AC3:AC6"/>
     <mergeCell ref="AB3:AB6"/>
     <mergeCell ref="AA3:AA6"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="N24:N26"/>
-    <mergeCell ref="M24:M26"/>
-    <mergeCell ref="L24:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>